<commit_message>
ADD UNIQUE AND AUTOINCREMENT
</commit_message>
<xml_diff>
--- a/cars-database.xlsx
+++ b/cars-database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanse\Desktop\ALL\ESERCIZI\db-first\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4446B9A-9B93-4D27-ABCB-7F935621B5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AA2A97-B1C3-4478-8930-EA576AE8C87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16305" yWindow="1335" windowWidth="16410" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14535" yWindow="-9330" windowWidth="12150" windowHeight="20685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Car ID</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>NOT NULL,UNIQUE</t>
+  </si>
+  <si>
+    <t>NOT NULL,AUTOINCREMENT,UNIQUE</t>
   </si>
 </sst>
 </file>
@@ -237,7 +240,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -520,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,7 +532,7 @@
     <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.44140625" customWidth="1"/>
     <col min="3" max="3" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.21875" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -558,7 +561,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>16</v>

</xml_diff>